<commit_message>
Added the login and register funtionality testing
</commit_message>
<xml_diff>
--- a/Test_Scenarios_and_Test_Cases_and_BugReport.xlsx
+++ b/Test_Scenarios_and_Test_Cases_and_BugReport.xlsx
@@ -8,25 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8472eb502463460a/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{62C90712-148B-4F1D-972E-A70A530880EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{466B4FEF-15B7-4357-BD2D-E6199DB93D06}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{62C90712-148B-4F1D-972E-A70A530880EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{95BACD0A-3C69-4FF0-882D-FF1A15B5161A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarios" sheetId="1" r:id="rId1"/>
-    <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
-    <sheet name="Bug Report" sheetId="3" r:id="rId3"/>
+    <sheet name="Form TestCases" sheetId="2" r:id="rId2"/>
+    <sheet name="LoginTescases" sheetId="4" r:id="rId3"/>
+    <sheet name="Register TestCases" sheetId="5" r:id="rId4"/>
+    <sheet name="Alert_Frame_window_TestCases" sheetId="6" r:id="rId5"/>
+    <sheet name="Bug Report" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="277">
   <si>
     <t>Scenario ID</t>
   </si>
   <si>
+    <t>SC001</t>
+  </si>
+  <si>
     <t>SC002</t>
   </si>
   <si>
@@ -36,12 +42,6 @@
     <t>SC004</t>
   </si>
   <si>
-    <t>SC005</t>
-  </si>
-  <si>
-    <t>SC006</t>
-  </si>
-  <si>
     <t>Test Case ID</t>
   </si>
   <si>
@@ -201,6 +201,9 @@
     <t>Validation errors shown</t>
   </si>
   <si>
+    <t>TC021</t>
+  </si>
+  <si>
     <t>Test Scenario Title</t>
   </si>
   <si>
@@ -232,12 +235,6 @@
   </si>
   <si>
     <t xml:space="preserve">Validate all the form elements of practice form </t>
-  </si>
-  <si>
-    <t>Elements</t>
-  </si>
-  <si>
-    <t>Validate the working of elements like textbox,radio button,etc.</t>
   </si>
   <si>
     <t>Alerts,Frame and Window</t>
@@ -500,13 +497,373 @@
   </si>
   <si>
     <t>Form should adjust correctly for smaller screens</t>
+  </si>
+  <si>
+    <t>Test Case Title</t>
+  </si>
+  <si>
+    <t>Login with valid credentials</t>
+  </si>
+  <si>
+    <t>Enter valid username and password, click login</t>
+  </si>
+  <si>
+    <t>Username: testuser</t>
+  </si>
+  <si>
+    <t>Password: Test@123</t>
+  </si>
+  <si>
+    <t>User should be logged in and redirected to the homepage</t>
+  </si>
+  <si>
+    <t>TC022</t>
+  </si>
+  <si>
+    <t>Login with invalid password</t>
+  </si>
+  <si>
+    <t>Enter valid username and incorrect password, click login</t>
+  </si>
+  <si>
+    <t>Password: wrongpass</t>
+  </si>
+  <si>
+    <t>Error message "Invalid credentials" should be displayed</t>
+  </si>
+  <si>
+    <t>TC023</t>
+  </si>
+  <si>
+    <t>Login with empty fields</t>
+  </si>
+  <si>
+    <t>Click login without entering any credentials</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>Validation messages for both fields should be displayed</t>
+  </si>
+  <si>
+    <t>TC024</t>
+  </si>
+  <si>
+    <t>Login with invalid email format</t>
+  </si>
+  <si>
+    <t>Enter invalid email format and valid password, click login</t>
+  </si>
+  <si>
+    <t>Email: testuser.com</t>
+  </si>
+  <si>
+    <t>Error: "Enter a valid email"</t>
+  </si>
+  <si>
+    <t>TC025</t>
+  </si>
+  <si>
+    <t>Login with SQL injection attempt</t>
+  </si>
+  <si>
+    <t>Try SQL injection in username or password fields</t>
+  </si>
+  <si>
+    <t>' OR '1'='1</t>
+  </si>
+  <si>
+    <t>Password: anything</t>
+  </si>
+  <si>
+    <t>Login should fail, input should be sanitized</t>
+  </si>
+  <si>
+    <t>TC026</t>
+  </si>
+  <si>
+    <t>Password field should be masked</t>
+  </si>
+  <si>
+    <t>Observe input while typing in password field</t>
+  </si>
+  <si>
+    <t>Password: any</t>
+  </si>
+  <si>
+    <t>Characters should be masked (e.g., ●●●●●)</t>
+  </si>
+  <si>
+    <t>TC027</t>
+  </si>
+  <si>
+    <t>Login button disabled when fields are empty</t>
+  </si>
+  <si>
+    <t>Try clicking login without entering data</t>
+  </si>
+  <si>
+    <t>Login button should be disabled or show validation messages</t>
+  </si>
+  <si>
+    <t>TC028</t>
+  </si>
+  <si>
+    <t>TC029</t>
+  </si>
+  <si>
+    <t>TC030</t>
+  </si>
+  <si>
+    <t>Register with valid inputs</t>
+  </si>
+  <si>
+    <t>Fill all fields with valid data and click Register</t>
+  </si>
+  <si>
+    <t>User should be registered and redirected</t>
+  </si>
+  <si>
+    <t>Register with existing username</t>
+  </si>
+  <si>
+    <t>Use a username that already exists</t>
+  </si>
+  <si>
+    <t>Register with blank fields</t>
+  </si>
+  <si>
+    <t>Click register with all fields empty</t>
+  </si>
+  <si>
+    <t>Validation errors should appear</t>
+  </si>
+  <si>
+    <t>TC031</t>
+  </si>
+  <si>
+    <t>Register with short password</t>
+  </si>
+  <si>
+    <t>Enter a password less than 6 characters</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>Validation error for password</t>
+  </si>
+  <si>
+    <t>TC032</t>
+  </si>
+  <si>
+    <t>Register with weak password (no special char)</t>
+  </si>
+  <si>
+    <t>Use only letters/numbers in password</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>TC033</t>
+  </si>
+  <si>
+    <t>Register with long username</t>
+  </si>
+  <si>
+    <t>Enter username longer than 50 characters</t>
+  </si>
+  <si>
+    <t>verylongusername...</t>
+  </si>
+  <si>
+    <t>Username field truncates or error shown</t>
+  </si>
+  <si>
+    <t>TC034</t>
+  </si>
+  <si>
+    <t>Register with only First Name filled</t>
+  </si>
+  <si>
+    <t>Fill only First Name and click Register</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Validation errors for other fields</t>
+  </si>
+  <si>
+    <t>TC035</t>
+  </si>
+  <si>
+    <t>Register with invalid characters in username</t>
+  </si>
+  <si>
+    <t>Use special characters in username</t>
+  </si>
+  <si>
+    <t>user!@#</t>
+  </si>
+  <si>
+    <t>TC036</t>
+  </si>
+  <si>
+    <t>Password should be masked</t>
+  </si>
+  <si>
+    <t>UI Test</t>
+  </si>
+  <si>
+    <t>Observe the password field</t>
+  </si>
+  <si>
+    <t>Password input should be masked</t>
+  </si>
+  <si>
+    <t>TC037</t>
+  </si>
+  <si>
+    <t>Confirm Registration redirects to login</t>
+  </si>
+  <si>
+    <t>Register successfully</t>
+  </si>
+  <si>
+    <t>Valid data</t>
+  </si>
+  <si>
+    <t>Redirects to login page</t>
+  </si>
+  <si>
+    <t>TC038</t>
+  </si>
+  <si>
+    <t>Responsive layout of registration form</t>
+  </si>
+  <si>
+    <t>Resize browser window and check responsiveness</t>
+  </si>
+  <si>
+    <t>Form adjusts to mobile/tablet views</t>
+  </si>
+  <si>
+    <t>Password strength warning should be shown</t>
+  </si>
+  <si>
+    <t>Anusha, Test, anushatest, Pass@123</t>
+  </si>
+  <si>
+    <t>anushatest</t>
+  </si>
+  <si>
+    <t>Error: “User exists!” should appear</t>
+  </si>
+  <si>
+    <t>Validate opening of new tab</t>
+  </si>
+  <si>
+    <t>Click on “New Tab” button</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>A new tab should open with the expected content</t>
+  </si>
+  <si>
+    <t>Validate opening of new window</t>
+  </si>
+  <si>
+    <t>Click on “New Window” button</t>
+  </si>
+  <si>
+    <t>A new browser window should open with the expected content</t>
+  </si>
+  <si>
+    <t>Validate alert popup display</t>
+  </si>
+  <si>
+    <t>Click on “Click me” button under Alerts section</t>
+  </si>
+  <si>
+    <t>An alert popup should be displayed</t>
+  </si>
+  <si>
+    <t>Validate alert confirmation text</t>
+  </si>
+  <si>
+    <t>Click on “Confirm Box” and click OK</t>
+  </si>
+  <si>
+    <t>Alert should close and confirmation text should be shown on the page</t>
+  </si>
+  <si>
+    <t>Validate prompt alert with input</t>
+  </si>
+  <si>
+    <t>Click on “Prompt Box”, enter text in alert, and click OK</t>
+  </si>
+  <si>
+    <t>"John"</t>
+  </si>
+  <si>
+    <t>The entered text should be displayed on the page</t>
+  </si>
+  <si>
+    <t>Validate small modal dialog opens</t>
+  </si>
+  <si>
+    <t>Click on “Small Modal” button</t>
+  </si>
+  <si>
+    <t>A small modal dialog should open with appropriate content</t>
+  </si>
+  <si>
+    <t>Validate large modal dialog opens</t>
+  </si>
+  <si>
+    <t>Click on “Large Modal” button</t>
+  </si>
+  <si>
+    <t>A large modal dialog should open with appropriate content</t>
+  </si>
+  <si>
+    <t>Validate closing of modal dialogs</t>
+  </si>
+  <si>
+    <t>Open modal, then click “Close” or “×” button</t>
+  </si>
+  <si>
+    <t>The modal should close</t>
+  </si>
+  <si>
+    <t>Alert should not accept input when disabled</t>
+  </si>
+  <si>
+    <t>Try interacting with alert buttons when JavaScript is disabled</t>
+  </si>
+  <si>
+    <t>Alert should not appear or interaction fails gracefully</t>
+  </si>
+  <si>
+    <t>Validate multiple tab handling</t>
+  </si>
+  <si>
+    <t>Click “New Tab” multiple times in succession</t>
+  </si>
+  <si>
+    <t>Each tab should open separately with the same content</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,8 +901,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -561,6 +934,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,7 +992,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -631,9 +1010,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -658,6 +1034,23 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -665,6 +1058,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -969,10 +1371,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="121" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1006,13 +1408,13 @@
       <c r="C2" t="s">
         <v>64</v>
       </c>
-      <c r="D2">
-        <v>1</v>
+      <c r="D2" s="16">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>66</v>
@@ -1020,13 +1422,13 @@
       <c r="C3" t="s">
         <v>67</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>68</v>
@@ -1034,41 +1436,22 @@
       <c r="C4" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D4">
-        <v>3</v>
+      <c r="D4" s="16">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="16">
         <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1081,494 +1464,494 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.109375" customWidth="1"/>
     <col min="2" max="2" width="9.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" style="7" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="31.44140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="43.44140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="33.33203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="31.44140625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="43.44140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:7" s="10" customFormat="1" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="13" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+    </row>
+    <row r="2" spans="1:7" s="12" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="E3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="E4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="F5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>83</v>
+      <c r="G5" s="7" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>85</v>
+      <c r="G6" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>81</v>
+      <c r="G7" s="7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="F8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="G9" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>95</v>
+      <c r="G10" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="8" t="s">
+      <c r="G12" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>101</v>
+      <c r="G13" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>110</v>
+      <c r="G16" s="7" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F17" s="8" t="s">
+      <c r="G17" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F18" s="8" t="s">
+      <c r="G18" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>114</v>
+        <v>3</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>117</v>
+        <v>14</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>156</v>
+        <v>3</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>154</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16" t="s">
-        <v>56</v>
+        <v>12</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>157</v>
+        <v>3</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="D22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>58</v>
+        <v>14</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D24" t="s">
+        <v>152</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="D24" t="s">
-        <v>154</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>158</v>
+      <c r="G24" s="15" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1581,6 +1964,896 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE1A348-8AD3-440D-9521-CA48BFAFD739}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="19"/>
+    <col min="2" max="2" width="16.5546875" style="19" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="19" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="27.21875" style="19" customWidth="1"/>
+    <col min="6" max="6" width="36.88671875" style="19" customWidth="1"/>
+    <col min="7" max="7" width="35" style="19" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="G3" s="22"/>
+    </row>
+    <row r="4" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="G8" s="22"/>
+    </row>
+    <row r="9" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="22"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="G10" s="22"/>
+    </row>
+    <row r="11" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+    </row>
+    <row r="15" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="22"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="22"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="22"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D54D6A92-6607-45C6-96EA-712AB1F909B5}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView zoomScale="81" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" customWidth="1"/>
+    <col min="6" max="6" width="28.109375" customWidth="1"/>
+    <col min="7" max="7" width="45.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A5" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="54" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>219</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>220</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="54" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A10" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>230</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>233</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+      <c r="A12" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>238</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18" t="s">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FD1D24-602E-4B7D-ABAA-DA169FDC0B1B}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="28"/>
+    <col min="3" max="3" width="23.33203125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="26.77734375" style="28" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="28"/>
+    <col min="7" max="7" width="33.88671875" style="28" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="F2" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>250</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>252</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>253</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="G4" s="27" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>256</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="G5" s="27" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="G7" s="27" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>265</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>268</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>269</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="D10" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>247</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>276</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC5F4EB8-6E11-4D9E-98F1-29515131D6FA}">
   <dimension ref="A1:I11"/>
   <sheetViews>
@@ -1598,229 +2871,215 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="E1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="H1" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="14"/>
+    </row>
+    <row r="2" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="E1" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="15" t="s">
+      <c r="B2" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="I1" s="15"/>
-    </row>
-    <row r="2" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="C2" s="23" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="E2" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="23"/>
+    </row>
+    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="23"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+    </row>
+    <row r="5" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="E2" s="17" t="s">
+      <c r="C5" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="G2" s="17" t="s">
+      <c r="I5" s="23"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+    </row>
+    <row r="7" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="I2" s="17"/>
-    </row>
-    <row r="3" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-    </row>
-    <row r="5" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="I5" s="17"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-    </row>
-    <row r="7" spans="1:9" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C7" s="17" t="s">
+      <c r="I7" s="23"/>
+    </row>
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="I7" s="17"/>
-    </row>
-    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
     </row>
     <row r="9" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>140</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="E9" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="E9" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="H9" s="18" t="s">
+      <c r="F9" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="24" t="s">
         <v>129</v>
       </c>
+      <c r="H9" s="24" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="24"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="I2:I4"/>
     <mergeCell ref="A5:A6"/>
@@ -1837,6 +3096,20 @@
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="G2:G4"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="G7:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added the login and register fuctionality testing
</commit_message>
<xml_diff>
--- a/Test_Scenarios_and_Test_Cases_and_BugReport.xlsx
+++ b/Test_Scenarios_and_Test_Cases_and_BugReport.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8472eb502463460a/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="8_{62C90712-148B-4F1D-972E-A70A530880EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{95BACD0A-3C69-4FF0-882D-FF1A15B5161A}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="8_{62C90712-148B-4F1D-972E-A70A530880EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{367B0D5F-33D1-468D-9AD9-EC2BE35E9AB6}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarios" sheetId="1" r:id="rId1"/>
     <sheet name="Form TestCases" sheetId="2" r:id="rId2"/>
     <sheet name="LoginTescases" sheetId="4" r:id="rId3"/>
     <sheet name="Register TestCases" sheetId="5" r:id="rId4"/>
-    <sheet name="Alert_Frame_window_TestCases" sheetId="6" r:id="rId5"/>
-    <sheet name="Bug Report" sheetId="3" r:id="rId6"/>
+    <sheet name="Bug Report" sheetId="3" r:id="rId5"/>
+    <sheet name="Alert_Frame_window_TestCases" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -808,9 +808,6 @@
     <t>Click on “Prompt Box”, enter text in alert, and click OK</t>
   </si>
   <si>
-    <t>"John"</t>
-  </si>
-  <si>
     <t>The entered text should be displayed on the page</t>
   </si>
   <si>
@@ -857,22 +854,17 @@
   </si>
   <si>
     <t>Each tab should open separately with the same content</t>
+  </si>
+  <si>
+    <t>"hello"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -917,8 +909,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -940,6 +947,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -990,9 +1003,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1000,13 +1013,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1014,40 +1027,42 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1059,15 +1074,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1374,7 +1388,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView zoomScale="121" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1408,7 +1422,7 @@
       <c r="C2" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="15">
         <v>3</v>
       </c>
     </row>
@@ -1422,7 +1436,7 @@
       <c r="C3" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="16">
+      <c r="D3" s="15">
         <v>2</v>
       </c>
     </row>
@@ -1436,7 +1450,7 @@
       <c r="C4" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="16">
+      <c r="D4" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1450,7 +1464,7 @@
       <c r="C5" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="15">
         <v>4</v>
       </c>
     </row>
@@ -1464,8 +1478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1538,7 +1552,7 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="13" t="s">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -1900,17 +1914,17 @@
       <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="14" t="s">
         <v>154</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15" t="s">
+      <c r="F21" s="14"/>
+      <c r="G21" s="14" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1950,13 +1964,14 @@
       <c r="E24" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="14" t="s">
         <v>156</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" location="'Test Scenarios'!A1" display="SC003" xr:uid="{199E2E80-BC25-4055-A56F-DFFD13B6B9B9}"/>
+    <hyperlink ref="B4" location="'Test Scenarios'!A1" display="SC003" xr:uid="{00B18138-B3BE-4412-8F29-0F25111248F8}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1968,41 +1983,41 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView zoomScale="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C8"/>
+      <selection activeCell="B15" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="19"/>
-    <col min="2" max="2" width="16.5546875" style="19" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" style="19" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" style="19" customWidth="1"/>
-    <col min="5" max="5" width="27.21875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="36.88671875" style="19" customWidth="1"/>
-    <col min="7" max="7" width="35" style="19" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="19"/>
+    <col min="1" max="1" width="8.88671875" style="18"/>
+    <col min="2" max="2" width="16.5546875" style="18" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="27.21875" style="18" customWidth="1"/>
+    <col min="6" max="6" width="36.88671875" style="18" customWidth="1"/>
+    <col min="7" max="7" width="35" style="18" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7" s="27" customFormat="1" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="26" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2022,7 +2037,7 @@
       <c r="E2" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>160</v>
       </c>
       <c r="G2" s="22" t="s">
@@ -2035,7 +2050,7 @@
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
       <c r="E3" s="22"/>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>161</v>
       </c>
       <c r="G3" s="22"/>
@@ -2056,7 +2071,7 @@
       <c r="E4" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>160</v>
       </c>
       <c r="G4" s="22" t="s">
@@ -2069,31 +2084,31 @@
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
       <c r="E5" s="22"/>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>166</v>
       </c>
       <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="17" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2113,7 +2128,7 @@
       <c r="E7" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>176</v>
       </c>
       <c r="G7" s="22" t="s">
@@ -2126,7 +2141,7 @@
       <c r="C8" s="22"/>
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="17" t="s">
         <v>161</v>
       </c>
       <c r="G8" s="22"/>
@@ -2147,7 +2162,7 @@
       <c r="E9" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="17" t="s">
         <v>181</v>
       </c>
       <c r="G9" s="22" t="s">
@@ -2160,72 +2175,72 @@
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="17" t="s">
         <v>182</v>
       </c>
       <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>185</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="17" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>189</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18" t="s">
+      <c r="F12" s="17"/>
+      <c r="G12" s="17" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
     </row>
     <row r="15" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="22"/>
@@ -2233,7 +2248,7 @@
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
       <c r="E15" s="22"/>
-      <c r="F15" s="18"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="22"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -2242,17 +2257,23 @@
       <c r="C16" s="22"/>
       <c r="D16" s="22"/>
       <c r="E16" s="22"/>
-      <c r="F16" s="18"/>
+      <c r="F16" s="17"/>
       <c r="G16" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
@@ -2265,18 +2286,12 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2300,272 +2315,272 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="36" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="17" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="36" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="17" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="36" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="17" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="54" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>209</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="17" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="36" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="17" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="36" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="17" t="s">
         <v>218</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="17" t="s">
         <v>221</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="17" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="54" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>224</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="17" t="s">
         <v>225</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="36" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>227</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>228</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="17" t="s">
         <v>230</v>
       </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18" t="s">
+      <c r="F10" s="17"/>
+      <c r="G10" s="17" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="36" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>233</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="17" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="36" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="17" t="s">
         <v>229</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18" t="s">
+      <c r="F12" s="17"/>
+      <c r="G12" s="17" t="s">
         <v>240</v>
       </c>
     </row>
@@ -2576,289 +2591,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FD1D24-602E-4B7D-ABAA-DA169FDC0B1B}">
-  <dimension ref="A1:G11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="2" width="8.88671875" style="28"/>
-    <col min="3" max="3" width="23.33203125" style="28" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="28" customWidth="1"/>
-    <col min="5" max="5" width="26.77734375" style="28" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" style="28"/>
-    <col min="7" max="7" width="33.88671875" style="28" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="28"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>157</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>245</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="G2" s="27" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>249</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>250</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="G3" s="27" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>252</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>253</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="G4" s="27" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>255</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>256</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="G5" s="27" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>258</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>259</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>260</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>262</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>265</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>266</v>
-      </c>
-      <c r="F8" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="G8" s="27" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>268</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="27" t="s">
-        <v>269</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>271</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="27" t="s">
-        <v>272</v>
-      </c>
-      <c r="F10" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="G10" s="27" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>275</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="G11" s="27" t="s">
-        <v>276</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC5F4EB8-6E11-4D9E-98F1-29515131D6FA}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2870,32 +2607,32 @@
     <col min="6" max="6" width="26.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:9" s="29" customFormat="1" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="14"/>
+      <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:9" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
@@ -2907,7 +2644,7 @@
       <c r="C2" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>123</v>
       </c>
       <c r="E2" s="23" t="s">
@@ -2928,7 +2665,7 @@
       <c r="A3" s="23"/>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>140</v>
       </c>
       <c r="E3" s="23"/>
@@ -2941,7 +2678,7 @@
       <c r="A4" s="23"/>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>124</v>
       </c>
       <c r="E4" s="23"/>
@@ -2960,7 +2697,7 @@
       <c r="C5" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>123</v>
       </c>
       <c r="E5" s="23" t="s">
@@ -2981,7 +2718,7 @@
       <c r="A6" s="23"/>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>143</v>
       </c>
       <c r="E6" s="23"/>
@@ -3000,7 +2737,7 @@
       <c r="C7" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>133</v>
       </c>
       <c r="E7" s="23" t="s">
@@ -3021,7 +2758,7 @@
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>134</v>
       </c>
       <c r="E8" s="23"/>
@@ -3040,7 +2777,7 @@
       <c r="C9" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="14" t="s">
         <v>146</v>
       </c>
       <c r="E9" s="24" t="s">
@@ -3059,7 +2796,7 @@
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>147</v>
       </c>
       <c r="E10" s="24"/>
@@ -3070,7 +2807,7 @@
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>124</v>
       </c>
       <c r="E11" s="24"/>
@@ -3080,6 +2817,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="I2:I4"/>
     <mergeCell ref="A5:A6"/>
@@ -3096,21 +2847,285 @@
     <mergeCell ref="E2:E4"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="G2:G4"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="G9:G11"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="G7:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FD1D24-602E-4B7D-ABAA-DA169FDC0B1B}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="21"/>
+    <col min="3" max="3" width="23.33203125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="26.77734375" style="21" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="21"/>
+    <col min="7" max="7" width="33.88671875" style="21" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>245</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>249</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>250</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>259</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>276</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>261</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>262</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>264</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>265</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>267</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>275</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>